<commit_message>
Started Section 'BIG DATA ANALYTICS'
</commit_message>
<xml_diff>
--- a/WordCount.xlsx
+++ b/WordCount.xlsx
@@ -413,7 +413,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Summary of Big Data Analysis completed [236 words]
</commit_message>
<xml_diff>
--- a/WordCount.xlsx
+++ b/WordCount.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,9 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -470,18 +468,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>200</v>
@@ -492,7 +490,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>200</v>
@@ -503,10 +501,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -544,7 +542,7 @@
       </c>
       <c r="C11" s="3">
         <f>SUM(C2:C10)</f>
-        <v>754</v>
+        <v>986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Warehousing complete, now all of Data Analytics completed
</commit_message>
<xml_diff>
--- a/WordCount.xlsx
+++ b/WordCount.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -224,6 +224,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -259,6 +276,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,13 +447,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -485,7 +521,7 @@
         <v>200</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>397</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -496,7 +532,7 @@
         <v>200</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -542,7 +578,7 @@
       </c>
       <c r="C11" s="3">
         <f>SUM(C2:C10)</f>
-        <v>986</v>
+        <v>1665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Benefits of Big Data completed
</commit_message>
<xml_diff>
--- a/WordCount.xlsx
+++ b/WordCount.xlsx
@@ -35,9 +35,6 @@
     <t>A Comprehensive look at Data</t>
   </si>
   <si>
-    <t>The Importance of Big Data</t>
-  </si>
-  <si>
     <t>Data Analytics</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>Actual Word Count</t>
+  </si>
+  <si>
+    <t>Benefits of Big Data</t>
   </si>
 </sst>
 </file>
@@ -447,9 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -460,13 +458,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,7 +502,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>200</v>
@@ -515,7 +513,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>200</v>
@@ -526,7 +524,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>200</v>
@@ -537,18 +535,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>300</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2">
         <v>300</v>
@@ -559,7 +557,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2">
         <v>200</v>
@@ -570,7 +568,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
         <f>SUM(B2:B10)</f>
@@ -578,7 +576,7 @@
       </c>
       <c r="C11" s="3">
         <f>SUM(C2:C10)</f>
-        <v>1665</v>
+        <v>1898</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Big Data, The next steps completed
</commit_message>
<xml_diff>
--- a/WordCount.xlsx
+++ b/WordCount.xlsx
@@ -447,7 +447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -552,7 +554,7 @@
         <v>300</v>
       </c>
       <c r="C9" s="2">
-        <v>0</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -576,7 +578,7 @@
       </c>
       <c r="C11" s="3">
         <f>SUM(C2:C10)</f>
-        <v>1898</v>
+        <v>2102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spell and Grammar check complete
</commit_message>
<xml_diff>
--- a/WordCount.xlsx
+++ b/WordCount.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Abstract</t>
   </si>
@@ -63,13 +63,16 @@
   </si>
   <si>
     <t>Benefits of Big Data</t>
+  </si>
+  <si>
+    <t>Final Word Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +88,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -94,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -117,11 +138,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -131,6 +180,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -579,6 +630,17 @@
         <v>2526</v>
       </c>
     </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="6">
+        <v>2583</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>